<commit_message>
End2End till RFV testing
</commit_message>
<xml_diff>
--- a/Resources/Testdata.xlsx
+++ b/Resources/Testdata.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0893DEA-03D9-4310-9234-478C467B778A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8233A6-6DD7-477D-9EA0-B4A28263CE2F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>User</t>
   </si>
@@ -59,13 +60,25 @@
   </si>
   <si>
     <t>Base</t>
+  </si>
+  <si>
+    <t>FTNames</t>
+  </si>
+  <si>
+    <t>DecnFT1</t>
+  </si>
+  <si>
+    <t>DecnFT2</t>
+  </si>
+  <si>
+    <t>DecnFT3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +92,14 @@
       <color rgb="FF008000"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,11 +122,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,10 +407,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9D28C0-9083-47FE-863A-84A28613A5E2}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>